<commit_message>
perbaikan error number format
</commit_message>
<xml_diff>
--- a/excel/contoh_bkk_infrastruktur.xlsx
+++ b/excel/contoh_bkk_infrastruktur.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="data pencairan" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
   <si>
     <t>no</t>
   </si>
@@ -265,6 +265,39 @@
   </si>
   <si>
     <t>RT 11 RW 21</t>
+  </si>
+  <si>
+    <t>import excel</t>
+  </si>
+  <si>
+    <t>RT 05</t>
+  </si>
+  <si>
+    <t>RT 27/ Rw 03 (Jl.Makam)</t>
+  </si>
+  <si>
+    <t>Banaran</t>
+  </si>
+  <si>
+    <t>RT 08 RW 02</t>
+  </si>
+  <si>
+    <t>kecamatan</t>
+  </si>
+  <si>
+    <t>kegiatan</t>
+  </si>
+  <si>
+    <t>realisasi</t>
+  </si>
+  <si>
+    <t>keterangan</t>
+  </si>
+  <si>
+    <t>Kec A</t>
+  </si>
+  <si>
+    <t>Desa A</t>
   </si>
 </sst>
 </file>
@@ -274,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,13 +346,31 @@
       <name val="Bookman Old Style"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -359,11 +410,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -418,10 +470,54 @@
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -716,7 +812,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1334,13 +1430,164 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="7" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75">
+      <c r="A1" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:8" ht="47.25">
+      <c r="A2" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="29">
+        <v>2023</v>
+      </c>
+      <c r="F2" s="30">
+        <v>60000000</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75">
+      <c r="A3" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="29">
+        <v>2023</v>
+      </c>
+      <c r="F3" s="30">
+        <v>50000000</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75">
+      <c r="A4" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="29">
+        <v>2023</v>
+      </c>
+      <c r="F4" s="30">
+        <v>50000000</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="23"/>
+    </row>
+    <row r="5" spans="1:8" ht="47.25">
+      <c r="A5" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="29">
+        <v>2023</v>
+      </c>
+      <c r="F5" s="30">
+        <v>150000000</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75">
+      <c r="A6" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="29">
+        <v>2023</v>
+      </c>
+      <c r="F6" s="30">
+        <v>100000000</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="23"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>